<commit_message>
UPDATE CONTENT:Add stage number
</commit_message>
<xml_diff>
--- a/OAMLab/161_运维观点/5205_运维.敏捷项目管理.企业软件研发效能DevSecOps工具集.流水线.示意图.20240701.2045.xlsx
+++ b/OAMLab/161_运维观点/5205_运维.敏捷项目管理.企业软件研发效能DevSecOps工具集.流水线.示意图.20240701.2045.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace_dev\java\GitHub_oamlab_001\OAMLab\161_运维观点\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA4FDF5-DBDA-42B9-B820-F5935116485F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B03139-66D1-49B8-8693-9EE1F8868B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10870" windowWidth="38620" windowHeight="21820" xr2:uid="{3DFADB1D-3BE0-4000-8963-FE3BE99B5F53}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>准备代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -327,6 +327,10 @@
   </si>
   <si>
     <t>runner-漏洞检查-Docker镜像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阶段：        1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -381,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -404,13 +408,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -433,14 +446,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,10 +784,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AG48"/>
+  <dimension ref="A2:AG49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -808,11 +833,11 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
@@ -955,577 +980,668 @@
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="16" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="12">
+        <v>2</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12">
+        <v>3</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="12">
+        <v>4</v>
+      </c>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="12">
+        <v>5</v>
+      </c>
+      <c r="O15" s="12"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="12">
+        <v>6</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="12">
+        <v>7</v>
+      </c>
+      <c r="U15" s="12"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="12">
+        <v>8</v>
+      </c>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="12">
+        <v>9</v>
+      </c>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="12">
+        <v>10</v>
+      </c>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="12">
+        <v>11</v>
+      </c>
+      <c r="AG15" s="12"/>
+    </row>
+    <row r="16" spans="1:33" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+    </row>
+    <row r="17" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="2" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="2" t="s">
+      <c r="F17" s="9"/>
+      <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="2" t="s">
+      <c r="I17" s="9"/>
+      <c r="J17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="M16" s="2" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N17" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="O16" s="8"/>
-      <c r="P16" s="2" t="s">
+      <c r="O17" s="9"/>
+      <c r="P17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q16" s="8" t="s">
+      <c r="Q17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="R16" s="8"/>
-      <c r="S16" s="2" t="s">
+      <c r="R17" s="9"/>
+      <c r="S17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T16" s="8" t="s">
+      <c r="T17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="U16" s="8"/>
-      <c r="V16" s="2" t="s">
+      <c r="U17" s="9"/>
+      <c r="V17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W16" s="8" t="s">
+      <c r="W17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="2" t="s">
+      <c r="X17" s="9"/>
+      <c r="Y17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Z16" s="8" t="s">
+      <c r="Z17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="2" t="s">
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AC16" s="8" t="s">
+      <c r="AC17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="2" t="s">
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AF16" s="8" t="s">
+      <c r="AF17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AG16" s="8"/>
-    </row>
-    <row r="17" spans="1:33" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="1">
-        <v>1</v>
-      </c>
-      <c r="O18" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>1</v>
-      </c>
-      <c r="R18" t="s">
-        <v>22</v>
-      </c>
-      <c r="T18" s="1">
-        <v>1</v>
-      </c>
-      <c r="U18" t="s">
-        <v>12</v>
-      </c>
-      <c r="W18" s="1">
-        <v>1</v>
-      </c>
-      <c r="X18" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>33</v>
-      </c>
+      <c r="AG17" s="9"/>
+    </row>
+    <row r="18" spans="1:33" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q19" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>22</v>
+      </c>
       <c r="T19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="W19" s="1">
+        <v>1</v>
+      </c>
+      <c r="X19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>33</v>
       </c>
       <c r="AC19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD19" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE19" s="1"/>
+        <v>33</v>
+      </c>
       <c r="AF19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>10</v>
+      </c>
       <c r="K20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N20" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O20" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="T20" s="1">
+        <v>2</v>
+      </c>
+      <c r="U20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="U20" t="s">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21" s="1">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="T21" s="1">
+        <v>3</v>
+      </c>
+      <c r="U21" t="s">
         <v>14</v>
       </c>
-      <c r="AC20" s="1">
+      <c r="AC21" s="1">
         <v>3</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AD21" t="s">
         <v>30</v>
       </c>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="K21" s="1">
-        <v>4</v>
-      </c>
-      <c r="L21" t="s">
-        <v>55</v>
-      </c>
-      <c r="N21" s="1">
-        <v>4</v>
-      </c>
-      <c r="O21" t="s">
-        <v>11</v>
-      </c>
-      <c r="T21" s="1">
-        <v>4</v>
-      </c>
-      <c r="U21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1">
-        <v>4</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>31</v>
-      </c>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="N22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O22" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="T22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U22" t="s">
-        <v>25</v>
+        <v>57</v>
+      </c>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K23" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N23" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O23" t="s">
+        <v>66</v>
+      </c>
+      <c r="T23" s="1">
+        <v>5</v>
+      </c>
+      <c r="U23" t="s">
         <v>25</v>
-      </c>
-      <c r="T23" s="1">
-        <v>6</v>
-      </c>
-      <c r="U23" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K24" s="1">
-        <v>7</v>
-      </c>
-      <c r="L24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" s="1">
+        <v>6</v>
+      </c>
+      <c r="O24" t="s">
         <v>25</v>
       </c>
-      <c r="N24" s="1">
-        <v>7</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="T24" s="1">
+        <v>6</v>
+      </c>
+      <c r="U24" t="s">
         <v>26</v>
-      </c>
-      <c r="T24" s="1">
-        <v>7</v>
-      </c>
-      <c r="U24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K25" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="1">
+        <v>7</v>
+      </c>
+      <c r="O25" t="s">
         <v>26</v>
       </c>
-      <c r="N25" s="1">
-        <v>8</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="T25" s="1">
+        <v>7</v>
+      </c>
+      <c r="U25" t="s">
         <v>27</v>
-      </c>
-      <c r="T25" s="1">
-        <v>8</v>
-      </c>
-      <c r="U25" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K26" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="1">
+        <v>8</v>
+      </c>
+      <c r="O26" t="s">
         <v>27</v>
       </c>
-      <c r="N26" s="1">
-        <v>9</v>
-      </c>
-      <c r="O26" t="s">
+      <c r="T26" s="1">
+        <v>8</v>
+      </c>
+      <c r="U26" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="K27" s="1">
+        <v>9</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" s="1">
+        <v>9</v>
+      </c>
+      <c r="O27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="K28" s="1">
         <v>10</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AA29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AC29" s="3"/>
-      <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B32" s="1">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <v>5</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
         <v>10</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="1">
+      <c r="C47" s="7"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="31">
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="N15:O15"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="T16:U16"/>
+    <mergeCell ref="AF17:AG17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T17:U17"/>
     <mergeCell ref="A6:AG6"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Z15:AA15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AF15:AG15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>